<commit_message>
Añadido logout en CloseAllAplications, cambio de login de process a InitAllSetting
</commit_message>
<xml_diff>
--- a/Proyecto_Final_Dispatcher/Data/Config.xlsx
+++ b/Proyecto_Final_Dispatcher/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bgnte\Documents\Proyecto final\Personal\Proyecto Final\Proyecto_Final_\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bgnte\Documents\UiPath\workspace\Proyecto_Final_Dispatcher\Proyecto_Final_Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE4E78F0-2DC5-4485-AF01-83DB60EF4162}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84F3E189-B4E9-4A9B-9C5C-533A68FFBEA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5268" yWindow="2436" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="55">
   <si>
     <t>Name</t>
   </si>
@@ -177,13 +177,19 @@
     <t>C:\Users\bgnte\Downloads\Vendor List.xlsx</t>
   </si>
   <si>
-    <t>in_Vendor List</t>
-  </si>
-  <si>
     <t>C:\Vendors\Vendor List.xlsx</t>
   </si>
   <si>
     <t>in_Vendor</t>
+  </si>
+  <si>
+    <t>out_Vendors_Path</t>
+  </si>
+  <si>
+    <t>C:\Vendors</t>
+  </si>
+  <si>
+    <t>vendor_list_download_path</t>
   </si>
 </sst>
 </file>
@@ -579,7 +585,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -674,7 +680,7 @@
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B8" t="s">
         <v>49</v>
@@ -682,15 +688,19 @@
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A10" s="2"/>
-      <c r="B10" s="5"/>
+      <c r="A10" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>

<commit_message>
Añadido control de excepciones
</commit_message>
<xml_diff>
--- a/Proyecto_Final_Dispatcher/Data/Config.xlsx
+++ b/Proyecto_Final_Dispatcher/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bgnte\Documents\UiPath\workspace\Proyecto_Final_Dispatcher\Proyecto_Final_Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84F3E189-B4E9-4A9B-9C5C-533A68FFBEA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B50F6D33-83A5-4932-9274-FDABEFF8886C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5268" yWindow="2436" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -585,7 +585,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
No sé que se ha modificado
</commit_message>
<xml_diff>
--- a/Proyecto_Final_Dispatcher/Data/Config.xlsx
+++ b/Proyecto_Final_Dispatcher/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bgnte\Documents\UiPath\workspace\Proyecto_Final_Dispatcher\Proyecto_Final_Dispatcher\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B50F6D33-83A5-4932-9274-FDABEFF8886C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{632A8D71-DC7D-4283-9CE5-3D0E5E036BE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5676" yWindow="696" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -183,13 +183,13 @@
     <t>in_Vendor</t>
   </si>
   <si>
-    <t>out_Vendors_Path</t>
-  </si>
-  <si>
     <t>C:\Vendors</t>
   </si>
   <si>
     <t>vendor_list_download_path</t>
+  </si>
+  <si>
+    <t>in_Vendors_Path</t>
   </si>
 </sst>
 </file>
@@ -585,7 +585,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
@@ -680,7 +680,7 @@
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B8" t="s">
         <v>49</v>
@@ -696,10 +696,10 @@
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1">
       <c r="A10" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" t="s">
         <v>52</v>
-      </c>
-      <c r="B10" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>

</xml_diff>